<commit_message>
max simplified the new points list
</commit_message>
<xml_diff>
--- a/assets/List_AllInputs_MatEdits.xlsx
+++ b/assets/List_AllInputs_MatEdits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schra02155\PycharmProjects\hanson-bas\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11628EE2-CBE9-4C97-B3AB-98B5B446352C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5F7171-2AA3-4E73-BF01-20A3A0163F02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2160" yWindow="3960" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1596,8 +1596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R440"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A273" workbookViewId="0">
-      <selection activeCell="P287" sqref="P287"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>